<commit_message>
getting users during initial data load
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/prescriptions.xlsx
+++ b/src/main/resources/initialDataFiles/prescriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F1197F-64EB-45C1-A4A3-B0EE457EF662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD075EB3-AF46-49B7-B35B-42193C75DDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{D62EB2BE-1EF4-4692-9FA4-4C3CA6687488}"/>
   </bookViews>
@@ -99,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -109,6 +109,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +427,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -473,7 +474,7 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -485,5 +486,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
loading times from prescriptions.xlsx, no longer use sql.time, replaced with LocalDateTime and @Temporal=TIMESTAMP
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/prescriptions.xlsx
+++ b/src/main/resources/initialDataFiles/prescriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD075EB3-AF46-49B7-B35B-42193C75DDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674BE409-F624-4786-9EEA-C2C961C925BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{D62EB2BE-1EF4-4692-9FA4-4C3CA6687488}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t xml:space="preserve"> DOSE_MG</t>
-  </si>
-  <si>
-    <t>2022-04-22 10:34:53.44</t>
   </si>
 </sst>
 </file>
@@ -56,7 +53,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="169" formatCode="yyyy/mm/dd\ hh:mm:ss\.ss"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -99,17 +96,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +423,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -464,21 +460,21 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>3</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
+      <c r="E2" s="4">
+        <v>44673.44027777778</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44673.44027777778</v>
       </c>
       <c r="G2">
         <v>15</v>

</xml_diff>